<commit_message>
fix: WorkedHourPointing bot updated
</commit_message>
<xml_diff>
--- a/05 - WorkedHourPointing/ApontamentoDiego.xlsx
+++ b/05 - WorkedHourPointing/ApontamentoDiego.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mao8ct\Desktop\PyAutomateSAP\05 - WorkedHourPointing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655626B0-DCE6-402D-8A31-C7C0DC61F95C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50CA1E74-41F7-41B0-BCCD-0B3E6BC65C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C9D61577-ED6E-49E0-8DF4-9B4D2FEA07AE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{C9D61577-ED6E-49E0-8DF4-9B4D2FEA07AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,73 +36,124 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>LPs</t>
   </si>
   <si>
-    <t>LP044947</t>
-  </si>
-  <si>
-    <t>LP044879</t>
-  </si>
-  <si>
-    <t>LP044990</t>
-  </si>
-  <si>
-    <t>LP045276</t>
-  </si>
-  <si>
-    <t>LP045393</t>
-  </si>
-  <si>
-    <t>LP045858</t>
-  </si>
-  <si>
-    <t>LP045848</t>
-  </si>
-  <si>
-    <t>LP045808</t>
-  </si>
-  <si>
-    <t>LP046059</t>
-  </si>
-  <si>
-    <t>LP046058</t>
-  </si>
-  <si>
-    <t>LP046062</t>
-  </si>
-  <si>
-    <t>LP046089</t>
-  </si>
-  <si>
-    <t>LP046090</t>
-  </si>
-  <si>
-    <t>LP046091</t>
-  </si>
-  <si>
-    <t>LP045861</t>
-  </si>
-  <si>
-    <t>LP046093</t>
-  </si>
-  <si>
-    <t>LP046293</t>
-  </si>
-  <si>
-    <t>LP046361</t>
-  </si>
-  <si>
-    <t>LP046366</t>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>LP046642</t>
+  </si>
+  <si>
+    <t>LP046644</t>
+  </si>
+  <si>
+    <t>LP046538</t>
+  </si>
+  <si>
+    <t>LP046567</t>
+  </si>
+  <si>
+    <t>LP046537</t>
+  </si>
+  <si>
+    <t>LP046682</t>
+  </si>
+  <si>
+    <t>LP047226</t>
+  </si>
+  <si>
+    <t>LP046627</t>
+  </si>
+  <si>
+    <t>LP046620</t>
+  </si>
+  <si>
+    <t>LP047343</t>
+  </si>
+  <si>
+    <t>LP046889</t>
+  </si>
+  <si>
+    <t>LP046890</t>
+  </si>
+  <si>
+    <t>LP047396</t>
+  </si>
+  <si>
+    <t>LP046976</t>
+  </si>
+  <si>
+    <t>LP047400</t>
+  </si>
+  <si>
+    <t>LP046999</t>
+  </si>
+  <si>
+    <t>LP047448</t>
+  </si>
+  <si>
+    <t>LP047406</t>
+  </si>
+  <si>
+    <t>LP047975</t>
+  </si>
+  <si>
+    <t>LP047661</t>
+  </si>
+  <si>
+    <t>LP047654</t>
+  </si>
+  <si>
+    <t>LP047662</t>
+  </si>
+  <si>
+    <t>LP047697</t>
+  </si>
+  <si>
+    <t>LP047698</t>
+  </si>
+  <si>
+    <t>LP047664</t>
+  </si>
+  <si>
+    <t>LP047723</t>
+  </si>
+  <si>
+    <t>LP047733</t>
+  </si>
+  <si>
+    <t>LP047730</t>
+  </si>
+  <si>
+    <t>LP047727</t>
+  </si>
+  <si>
+    <t>LP047728</t>
+  </si>
+  <si>
+    <t>LP047978</t>
+  </si>
+  <si>
+    <t>LP048050</t>
+  </si>
+  <si>
+    <t>LP048185</t>
+  </si>
+  <si>
+    <t>LP048186</t>
+  </si>
+  <si>
+    <t>LP047956</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,25 +167,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -164,15 +209,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -193,9 +241,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -233,7 +281,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -339,7 +387,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -481,7 +529,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -489,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B67CD9C8-C549-42C7-8116-4422AAB55D3F}">
-  <dimension ref="A1:A58"/>
+  <dimension ref="A1:B58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,221 +548,257 @@
     <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
     </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>16</v>
+      <c r="A17" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>17</v>
+      <c r="A18" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>18</v>
+      <c r="A19" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>19</v>
+      <c r="A20" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
+      <c r="A21" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
+      <c r="A22" s="4" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
+      <c r="A23" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
+      <c r="A24" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
+      <c r="A25" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
+      <c r="A26" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
+      <c r="A27" s="4" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
+      <c r="A28" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
+      <c r="A29" s="4" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
+      <c r="A30" s="4" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
+      <c r="A31" s="4" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
+      <c r="A32" s="4" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
+      <c r="A33" s="4" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
+      <c r="A34" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
+      <c r="A35" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
+      <c r="A36" s="4" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
+      <c r="A37" s="1"/>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
+      <c r="A38" s="1"/>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
+      <c r="A39" s="1"/>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
+      <c r="A40" s="1"/>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
+      <c r="A41" s="1"/>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
+      <c r="A42" s="1"/>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
+      <c r="A43" s="1"/>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
+      <c r="A44" s="1"/>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="3"/>
+      <c r="A45" s="1"/>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="3"/>
+      <c r="A46" s="1"/>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="3"/>
+      <c r="A47" s="1"/>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="3"/>
+      <c r="A48" s="1"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="3"/>
+      <c r="A49" s="1"/>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="3"/>
+      <c r="A50" s="1"/>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="3"/>
+      <c r="A51" s="1"/>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="3"/>
+      <c r="A52" s="1"/>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="3"/>
+      <c r="A53" s="1"/>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="3"/>
+      <c r="A54" s="1"/>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="3"/>
+      <c r="A55" s="1"/>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="3"/>
+      <c r="A56" s="1"/>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="3"/>
+      <c r="A57" s="1"/>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="3"/>
+      <c r="A58" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>